<commit_message>
Plantilla de reporte y primeras dosfunciones completadas
</commit_message>
<xml_diff>
--- a/notas_estudiantes.xlsx
+++ b/notas_estudiantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etaln\Documents\Programacion\Python\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FCFED7-F358-41F6-937C-7327A15DF43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FAE348-59C2-40E2-84E5-4EE9335F0293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:B16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Se implementó la función 6 de la rama Kevin (CORREGIDO)
</commit_message>
<xml_diff>
--- a/notas_estudiantes.xlsx
+++ b/notas_estudiantes.xlsx
@@ -1,115 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etaln\Documents\Programacion\Python\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89364649-347A-415F-B683-E1DEA7D0F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="notas" sheetId="1" r:id="rId1"/>
+    <sheet name="notas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Reporte 2025-04-27 22-01-30" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Nombre del estudiante</t>
-  </si>
-  <si>
-    <t>Nota</t>
-  </si>
-  <si>
-    <t>Juan Carlos Ramírez Ortega</t>
-  </si>
-  <si>
-    <t>María Fernanda López Hernández</t>
-  </si>
-  <si>
-    <t>Luis Alejandro Torres Jiménez</t>
-  </si>
-  <si>
-    <t>Ana Sofía Castillo Pérez</t>
-  </si>
-  <si>
-    <t>Pedro Javier Mendoza Ruiz</t>
-  </si>
-  <si>
-    <t>Camila Teresa Vargas Morales</t>
-  </si>
-  <si>
-    <t>Diego Armando Soto Aguilar</t>
-  </si>
-  <si>
-    <t>Valeria Isabel Márquez Rivas</t>
-  </si>
-  <si>
-    <t>Andrés Felipe Gutiérrez Navarro</t>
-  </si>
-  <si>
-    <t>Daniela Alejandra Pineda Salazar</t>
-  </si>
-  <si>
-    <t>José Manuel Herrera Ponce</t>
-  </si>
-  <si>
-    <t>Karla Patricia Rodríguez Núñez</t>
-  </si>
-  <si>
-    <t>Sebastián Elías Cordero Romero</t>
-  </si>
-  <si>
-    <t>Lucía Beatriz Navarro Delgado</t>
-  </si>
-  <si>
-    <t>Rodrigo Antonio Peña Castañeda</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -142,31 +72,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -486,148 +478,333 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col width="20.109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="5" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Nombre del estudiante</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Nota</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="28.8" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Juan Carlos Ramírez Ortega</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
+    <row r="3" ht="28.8" customHeight="1">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>María Fernanda López Hernández</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
+    <row r="4" ht="28.8" customHeight="1">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Luis Alejandro Torres Jiménez</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="5" ht="28.8" customHeight="1">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Ana Sofía Castillo Pérez</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="6" ht="28.8" customHeight="1">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Pedro Javier Mendoza Ruiz</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
+    <row r="7" ht="28.8" customHeight="1">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Camila Teresa Vargas Morales</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="8" ht="28.8" customHeight="1">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Diego Armando Soto Aguilar</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="9" ht="28.8" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Valeria Isabel Márquez Rivas</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="10" ht="28.8" customHeight="1">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Andrés Felipe Gutiérrez Navarro</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="11" ht="28.8" customHeight="1">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Daniela Alejandra Pineda Salazar</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="12" ht="28.8" customHeight="1">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>José Manuel Herrera Ponce</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="13" ht="28.8" customHeight="1">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Karla Patricia Rodríguez Núñez</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2">
+    <row r="14" ht="28.8" customHeight="1">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Sebastián Elías Cordero Romero</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
+    <row r="15" ht="28.8" customHeight="1">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Lucía Beatriz Navarro Delgado</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
+    <row r="16" ht="28.8" customHeight="1">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Rodrigo Antonio Peña Castañeda</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Estadisticas</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Numeros</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Porcentajes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Numero total de estudiantes</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(notas!A2:A16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Numero de estudiantes aprobados (nota &gt;= 70)</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTIF(notas!B2:B16,"&gt;=70")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Porcentaje de estudiantes aprobados (nota &gt;= 70)</t>
+        </is>
+      </c>
+      <c r="C4" s="5">
+        <f>B3/B2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Numero de estudiantes reprobados (nota &lt; 70)</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTIF(notas!B2:B16,"&lt;70")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Porcentaje de estudiantes reprobados (nota &lt; 70)</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>B5</f>
+        <v/>
+      </c>
+      <c r="C6" s="5">
+        <f>B5/B2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Numero de estudiantes reprobados con notas entre 60 y 69</t>
+        </is>
+      </c>
+      <c r="B7">
+        <f>COUNTIFS(notas!B2:B16,"&gt;=60",notas!B2:B16,"&lt;70")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Porcentaje de estudiantes reprobados con notas entre 60 y 69</t>
+        </is>
+      </c>
+      <c r="B8">
+        <f>B7</f>
+        <v/>
+      </c>
+      <c r="C8" s="5">
+        <f>B7/B2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Media de las notas</t>
+        </is>
+      </c>
+      <c r="B9" s="6">
+        <f>AVERAGE(notas!B2:B16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Desviación estandar de las notas</t>
+        </is>
+      </c>
+      <c r="B10" s="6">
+        <f>STDEVP(notas!B2:B16)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Programa listo y corregido (creo)
</commit_message>
<xml_diff>
--- a/notas_estudiantes.xlsx
+++ b/notas_estudiantes.xlsx
@@ -1,115 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etaln\Documents\Programacion\Python\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0969B35F-BBF8-4580-847C-8C74C347CBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="notas" sheetId="1" r:id="rId1"/>
+    <sheet name="notas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Reporte 2025-04-27 23-10-53" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Nombre del estudiante</t>
-  </si>
-  <si>
-    <t>Nota</t>
-  </si>
-  <si>
-    <t>Juan Carlos Ramírez Ortega</t>
-  </si>
-  <si>
-    <t>María Fernanda López Hernández</t>
-  </si>
-  <si>
-    <t>Luis Alejandro Torres Jiménez</t>
-  </si>
-  <si>
-    <t>Ana Sofía Castillo Pérez</t>
-  </si>
-  <si>
-    <t>Pedro Javier Mendoza Ruiz</t>
-  </si>
-  <si>
-    <t>Camila Teresa Vargas Morales</t>
-  </si>
-  <si>
-    <t>Diego Armando Soto Aguilar</t>
-  </si>
-  <si>
-    <t>Valeria Isabel Márquez Rivas</t>
-  </si>
-  <si>
-    <t>Andrés Felipe Gutiérrez Navarro</t>
-  </si>
-  <si>
-    <t>Daniela Alejandra Pineda Salazar</t>
-  </si>
-  <si>
-    <t>José Manuel Herrera Ponce</t>
-  </si>
-  <si>
-    <t>Karla Patricia Rodríguez Núñez</t>
-  </si>
-  <si>
-    <t>Sebastián Elías Cordero Romero</t>
-  </si>
-  <si>
-    <t>Lucía Beatriz Navarro Delgado</t>
-  </si>
-  <si>
-    <t>Rodrigo Antonio Peña Castañeda</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -142,31 +72,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -486,148 +478,333 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col width="20.109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="5" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Nombre del estudiante</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Nota</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="28.8" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Juan Carlos Ramírez Ortega</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
+    <row r="3" ht="28.8" customHeight="1">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>María Fernanda López Hernández</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
+    <row r="4" ht="28.8" customHeight="1">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Luis Alejandro Torres Jiménez</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="5" ht="28.8" customHeight="1">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Ana Sofía Castillo Pérez</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="6" ht="28.8" customHeight="1">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Pedro Javier Mendoza Ruiz</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
+    <row r="7" ht="28.8" customHeight="1">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Camila Teresa Vargas Morales</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="8" ht="28.8" customHeight="1">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Diego Armando Soto Aguilar</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="9" ht="28.8" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Valeria Isabel Márquez Rivas</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="10" ht="28.8" customHeight="1">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Andrés Felipe Gutiérrez Navarro</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="11" ht="28.8" customHeight="1">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Daniela Alejandra Pineda Salazar</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="12" ht="28.8" customHeight="1">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>José Manuel Herrera Ponce</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="13" ht="28.8" customHeight="1">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Karla Patricia Rodríguez Núñez</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2">
+    <row r="14" ht="28.8" customHeight="1">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Sebastián Elías Cordero Romero</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
+    <row r="15" ht="28.8" customHeight="1">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Lucía Beatriz Navarro Delgado</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
+    <row r="16" ht="28.8" customHeight="1">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Rodrigo Antonio Peña Castañeda</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Estadisticas</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Numeros</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Porcentajes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Numero total de estudiantes</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(notas!A2:A16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Numero de estudiantes aprobados (nota &gt;= 70)</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTIF(notas!B2:B16,"&gt;=70")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Porcentaje de estudiantes aprobados (nota &gt;= 70)</t>
+        </is>
+      </c>
+      <c r="C4" s="5">
+        <f>B3/B2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Numero de estudiantes reprobados (nota &lt; 70)</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTIF(notas!B2:B16,"&lt;70")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Porcentaje de estudiantes reprobados (nota &lt; 70)</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>B5</f>
+        <v/>
+      </c>
+      <c r="C6" s="5">
+        <f>B5/B2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Numero de estudiantes reprobados con notas entre 60 y 69</t>
+        </is>
+      </c>
+      <c r="B7">
+        <f>COUNTIFS(notas!B2:B16,"&gt;=60",notas!B2:B16,"&lt;70")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Porcentaje de estudiantes reprobados con notas entre 60 y 69</t>
+        </is>
+      </c>
+      <c r="B8">
+        <f>B7</f>
+        <v/>
+      </c>
+      <c r="C8" s="5">
+        <f>B7/B2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Media de las notas</t>
+        </is>
+      </c>
+      <c r="B9" s="6">
+        <f>AVERAGE(notas!B2:B16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Desviación estandar de las notas</t>
+        </is>
+      </c>
+      <c r="B10" s="6">
+        <f>STDEVP(notas!B2:B16)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>